<commit_message>
Split Character Class, Added Commands
PLus a whole lot of shit basically overhauled some systems and did minute tweaking also added a parser to parse characters and some other stuff
</commit_message>
<xml_diff>
--- a/Move list.xlsx
+++ b/Move list.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="274">
   <si>
     <t>Move Name</t>
   </si>
@@ -577,7 +577,7 @@
     <t>The user creates a reflective barrier that protects them from physical attacks. The user gains resistance to physical damage for the next minute. If a physical attack hits the user during this time, the attacker takes damage equal to half the damage dealt (rounded down).</t>
   </si>
   <si>
-    <t>Make magic mirrior</t>
+    <t>apply status{reflect} for target in range{Allies:5}</t>
   </si>
   <si>
     <t>Poison Powder</t>
@@ -646,7 +646,7 @@
     <t>The user creates a powerful twister that hits all adjacent targets, possibly lifting them into the air. The targets must make a Strength saving throw or be lifted 5 feet into the air and take falling damage when they land.</t>
   </si>
   <si>
-    <t>Make additional damage</t>
+    <t>apply damage{25} if chance{33%} for target in range{Enemy:5}</t>
   </si>
   <si>
     <t>Agility</t>
@@ -821,6 +821,18 @@
   </si>
   <si>
     <t>apply weather{create:hail} for target in single{User}</t>
+  </si>
+  <si>
+    <t>Ember</t>
+  </si>
+  <si>
+    <t>Vine Whip</t>
+  </si>
+  <si>
+    <t>1d12 + 0.5 INT grass damage</t>
+  </si>
+  <si>
+    <t>Dragon Pride</t>
   </si>
 </sst>
 </file>
@@ -2741,6 +2753,75 @@
         <v>269</v>
       </c>
     </row>
+    <row r="73">
+      <c r="A73" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C73" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="G73" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C74" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="G74" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="G75" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>